<commit_message>
committing changes to save state
</commit_message>
<xml_diff>
--- a/Wakanda_interface_selectors.xlsx
+++ b/Wakanda_interface_selectors.xlsx
@@ -2136,7 +2136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2193,6 +2193,21 @@
           <t>default</t>
         </is>
       </c>
+      <c r="E2" s="62" t="n"/>
+      <c r="F2" s="62" t="n"/>
+      <c r="G2" s="62" t="n"/>
+      <c r="H2" s="62" t="n"/>
+      <c r="I2" s="62" t="n"/>
+      <c r="J2" s="62" t="n"/>
+      <c r="K2" s="62" t="n"/>
+      <c r="L2" s="62" t="n"/>
+      <c r="M2" s="62" t="n"/>
+      <c r="N2" s="62" t="n"/>
+      <c r="O2" s="62" t="inlineStr">
+        <is>
+          <t>vpc001</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="63" t="inlineStr">
@@ -2211,6 +2226,21 @@
         </is>
       </c>
       <c r="D3" s="63" t="n"/>
+      <c r="E3" s="63" t="n"/>
+      <c r="F3" s="63" t="n"/>
+      <c r="G3" s="63" t="n"/>
+      <c r="H3" s="63" t="n"/>
+      <c r="I3" s="63" t="n"/>
+      <c r="J3" s="63" t="n"/>
+      <c r="K3" s="63" t="n"/>
+      <c r="L3" s="63" t="n"/>
+      <c r="M3" s="63" t="n"/>
+      <c r="N3" s="63" t="n"/>
+      <c r="O3" s="63" t="inlineStr">
+        <is>
+          <t>vpc002</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="62" t="inlineStr">
@@ -2229,6 +2259,21 @@
         </is>
       </c>
       <c r="D4" s="62" t="n"/>
+      <c r="E4" s="62" t="n"/>
+      <c r="F4" s="62" t="n"/>
+      <c r="G4" s="62" t="n"/>
+      <c r="H4" s="62" t="n"/>
+      <c r="I4" s="62" t="n"/>
+      <c r="J4" s="62" t="n"/>
+      <c r="K4" s="62" t="n"/>
+      <c r="L4" s="62" t="n"/>
+      <c r="M4" s="62" t="n"/>
+      <c r="N4" s="62" t="n"/>
+      <c r="O4" s="62" t="inlineStr">
+        <is>
+          <t>vpc003</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="63" t="n"/>
@@ -2243,6 +2288,21 @@
         </is>
       </c>
       <c r="D5" s="63" t="n"/>
+      <c r="E5" s="63" t="n"/>
+      <c r="F5" s="63" t="n"/>
+      <c r="G5" s="63" t="n"/>
+      <c r="H5" s="63" t="n"/>
+      <c r="I5" s="63" t="n"/>
+      <c r="J5" s="63" t="n"/>
+      <c r="K5" s="63" t="n"/>
+      <c r="L5" s="63" t="n"/>
+      <c r="M5" s="63" t="n"/>
+      <c r="N5" s="63" t="n"/>
+      <c r="O5" s="63" t="inlineStr">
+        <is>
+          <t>vpc004</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="62" t="n"/>
@@ -2257,6 +2317,21 @@
         </is>
       </c>
       <c r="D6" s="62" t="n"/>
+      <c r="E6" s="62" t="n"/>
+      <c r="F6" s="62" t="n"/>
+      <c r="G6" s="62" t="n"/>
+      <c r="H6" s="62" t="n"/>
+      <c r="I6" s="62" t="n"/>
+      <c r="J6" s="62" t="n"/>
+      <c r="K6" s="62" t="n"/>
+      <c r="L6" s="62" t="n"/>
+      <c r="M6" s="62" t="n"/>
+      <c r="N6" s="62" t="n"/>
+      <c r="O6" s="62" t="inlineStr">
+        <is>
+          <t>vpc005</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="63" t="n"/>
@@ -2267,6 +2342,21 @@
         </is>
       </c>
       <c r="D7" s="63" t="n"/>
+      <c r="E7" s="63" t="n"/>
+      <c r="F7" s="63" t="n"/>
+      <c r="G7" s="63" t="n"/>
+      <c r="H7" s="63" t="n"/>
+      <c r="I7" s="63" t="n"/>
+      <c r="J7" s="63" t="n"/>
+      <c r="K7" s="63" t="n"/>
+      <c r="L7" s="63" t="n"/>
+      <c r="M7" s="63" t="n"/>
+      <c r="N7" s="63" t="n"/>
+      <c r="O7" s="63" t="inlineStr">
+        <is>
+          <t>vpc006</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="62" t="n"/>
@@ -2277,6 +2367,21 @@
         </is>
       </c>
       <c r="D8" s="62" t="n"/>
+      <c r="E8" s="62" t="n"/>
+      <c r="F8" s="62" t="n"/>
+      <c r="G8" s="62" t="n"/>
+      <c r="H8" s="62" t="n"/>
+      <c r="I8" s="62" t="n"/>
+      <c r="J8" s="62" t="n"/>
+      <c r="K8" s="62" t="n"/>
+      <c r="L8" s="62" t="n"/>
+      <c r="M8" s="62" t="n"/>
+      <c r="N8" s="62" t="n"/>
+      <c r="O8" s="62" t="inlineStr">
+        <is>
+          <t>vpc007</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="63" t="n"/>
@@ -2287,6 +2392,21 @@
         </is>
       </c>
       <c r="D9" s="63" t="n"/>
+      <c r="E9" s="63" t="n"/>
+      <c r="F9" s="63" t="n"/>
+      <c r="G9" s="63" t="n"/>
+      <c r="H9" s="63" t="n"/>
+      <c r="I9" s="63" t="n"/>
+      <c r="J9" s="63" t="n"/>
+      <c r="K9" s="63" t="n"/>
+      <c r="L9" s="63" t="n"/>
+      <c r="M9" s="63" t="n"/>
+      <c r="N9" s="63" t="n"/>
+      <c r="O9" s="63" t="inlineStr">
+        <is>
+          <t>vpc008</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="62" t="n"/>
@@ -2297,6 +2417,21 @@
         </is>
       </c>
       <c r="D10" s="62" t="n"/>
+      <c r="E10" s="62" t="n"/>
+      <c r="F10" s="62" t="n"/>
+      <c r="G10" s="62" t="n"/>
+      <c r="H10" s="62" t="n"/>
+      <c r="I10" s="62" t="n"/>
+      <c r="J10" s="62" t="n"/>
+      <c r="K10" s="62" t="n"/>
+      <c r="L10" s="62" t="n"/>
+      <c r="M10" s="62" t="n"/>
+      <c r="N10" s="62" t="n"/>
+      <c r="O10" s="62" t="inlineStr">
+        <is>
+          <t>vpc009</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="63" t="n"/>
@@ -2307,6 +2442,21 @@
         </is>
       </c>
       <c r="D11" s="63" t="n"/>
+      <c r="E11" s="63" t="n"/>
+      <c r="F11" s="63" t="n"/>
+      <c r="G11" s="63" t="n"/>
+      <c r="H11" s="63" t="n"/>
+      <c r="I11" s="63" t="n"/>
+      <c r="J11" s="63" t="n"/>
+      <c r="K11" s="63" t="n"/>
+      <c r="L11" s="63" t="n"/>
+      <c r="M11" s="63" t="n"/>
+      <c r="N11" s="63" t="n"/>
+      <c r="O11" s="63" t="inlineStr">
+        <is>
+          <t>vpc010</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="62" t="n"/>
@@ -2317,6 +2467,21 @@
         </is>
       </c>
       <c r="D12" s="62" t="n"/>
+      <c r="E12" s="62" t="n"/>
+      <c r="F12" s="62" t="n"/>
+      <c r="G12" s="62" t="n"/>
+      <c r="H12" s="62" t="n"/>
+      <c r="I12" s="62" t="n"/>
+      <c r="J12" s="62" t="n"/>
+      <c r="K12" s="62" t="n"/>
+      <c r="L12" s="62" t="n"/>
+      <c r="M12" s="62" t="n"/>
+      <c r="N12" s="62" t="n"/>
+      <c r="O12" s="62" t="inlineStr">
+        <is>
+          <t>vpc011</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="63" t="n"/>
@@ -2327,6 +2492,21 @@
         </is>
       </c>
       <c r="D13" s="63" t="n"/>
+      <c r="E13" s="63" t="n"/>
+      <c r="F13" s="63" t="n"/>
+      <c r="G13" s="63" t="n"/>
+      <c r="H13" s="63" t="n"/>
+      <c r="I13" s="63" t="n"/>
+      <c r="J13" s="63" t="n"/>
+      <c r="K13" s="63" t="n"/>
+      <c r="L13" s="63" t="n"/>
+      <c r="M13" s="63" t="n"/>
+      <c r="N13" s="63" t="n"/>
+      <c r="O13" s="63" t="inlineStr">
+        <is>
+          <t>vpc012</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="62" t="n"/>
@@ -2337,6 +2517,21 @@
         </is>
       </c>
       <c r="D14" s="62" t="n"/>
+      <c r="E14" s="62" t="n"/>
+      <c r="F14" s="62" t="n"/>
+      <c r="G14" s="62" t="n"/>
+      <c r="H14" s="62" t="n"/>
+      <c r="I14" s="62" t="n"/>
+      <c r="J14" s="62" t="n"/>
+      <c r="K14" s="62" t="n"/>
+      <c r="L14" s="62" t="n"/>
+      <c r="M14" s="62" t="n"/>
+      <c r="N14" s="62" t="n"/>
+      <c r="O14" s="62" t="inlineStr">
+        <is>
+          <t>vpc013</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="63" t="n"/>
@@ -2347,6 +2542,21 @@
         </is>
       </c>
       <c r="D15" s="63" t="n"/>
+      <c r="E15" s="63" t="n"/>
+      <c r="F15" s="63" t="n"/>
+      <c r="G15" s="63" t="n"/>
+      <c r="H15" s="63" t="n"/>
+      <c r="I15" s="63" t="n"/>
+      <c r="J15" s="63" t="n"/>
+      <c r="K15" s="63" t="n"/>
+      <c r="L15" s="63" t="n"/>
+      <c r="M15" s="63" t="n"/>
+      <c r="N15" s="63" t="n"/>
+      <c r="O15" s="63" t="inlineStr">
+        <is>
+          <t>vpc014</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="62" t="n"/>
@@ -2357,6 +2567,21 @@
         </is>
       </c>
       <c r="D16" s="62" t="n"/>
+      <c r="E16" s="62" t="n"/>
+      <c r="F16" s="62" t="n"/>
+      <c r="G16" s="62" t="n"/>
+      <c r="H16" s="62" t="n"/>
+      <c r="I16" s="62" t="n"/>
+      <c r="J16" s="62" t="n"/>
+      <c r="K16" s="62" t="n"/>
+      <c r="L16" s="62" t="n"/>
+      <c r="M16" s="62" t="n"/>
+      <c r="N16" s="62" t="n"/>
+      <c r="O16" s="62" t="inlineStr">
+        <is>
+          <t>vpc015</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="63" t="n"/>
@@ -2367,6 +2592,21 @@
         </is>
       </c>
       <c r="D17" s="63" t="n"/>
+      <c r="E17" s="63" t="n"/>
+      <c r="F17" s="63" t="n"/>
+      <c r="G17" s="63" t="n"/>
+      <c r="H17" s="63" t="n"/>
+      <c r="I17" s="63" t="n"/>
+      <c r="J17" s="63" t="n"/>
+      <c r="K17" s="63" t="n"/>
+      <c r="L17" s="63" t="n"/>
+      <c r="M17" s="63" t="n"/>
+      <c r="N17" s="63" t="n"/>
+      <c r="O17" s="63" t="inlineStr">
+        <is>
+          <t>vpc016</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="62" t="n"/>
@@ -2377,6 +2617,21 @@
         </is>
       </c>
       <c r="D18" s="62" t="n"/>
+      <c r="E18" s="62" t="n"/>
+      <c r="F18" s="62" t="n"/>
+      <c r="G18" s="62" t="n"/>
+      <c r="H18" s="62" t="n"/>
+      <c r="I18" s="62" t="n"/>
+      <c r="J18" s="62" t="n"/>
+      <c r="K18" s="62" t="n"/>
+      <c r="L18" s="62" t="n"/>
+      <c r="M18" s="62" t="n"/>
+      <c r="N18" s="62" t="n"/>
+      <c r="O18" s="62" t="inlineStr">
+        <is>
+          <t>vpc017</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="63" t="n"/>
@@ -2387,6 +2642,21 @@
         </is>
       </c>
       <c r="D19" s="63" t="n"/>
+      <c r="E19" s="63" t="n"/>
+      <c r="F19" s="63" t="n"/>
+      <c r="G19" s="63" t="n"/>
+      <c r="H19" s="63" t="n"/>
+      <c r="I19" s="63" t="n"/>
+      <c r="J19" s="63" t="n"/>
+      <c r="K19" s="63" t="n"/>
+      <c r="L19" s="63" t="n"/>
+      <c r="M19" s="63" t="n"/>
+      <c r="N19" s="63" t="n"/>
+      <c r="O19" s="63" t="inlineStr">
+        <is>
+          <t>vpc018</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="62" t="n"/>
@@ -2397,6 +2667,21 @@
         </is>
       </c>
       <c r="D20" s="62" t="n"/>
+      <c r="E20" s="62" t="n"/>
+      <c r="F20" s="62" t="n"/>
+      <c r="G20" s="62" t="n"/>
+      <c r="H20" s="62" t="n"/>
+      <c r="I20" s="62" t="n"/>
+      <c r="J20" s="62" t="n"/>
+      <c r="K20" s="62" t="n"/>
+      <c r="L20" s="62" t="n"/>
+      <c r="M20" s="62" t="n"/>
+      <c r="N20" s="62" t="n"/>
+      <c r="O20" s="62" t="inlineStr">
+        <is>
+          <t>vpc019</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="63" t="n"/>
@@ -2407,6 +2692,21 @@
         </is>
       </c>
       <c r="D21" s="63" t="n"/>
+      <c r="E21" s="63" t="n"/>
+      <c r="F21" s="63" t="n"/>
+      <c r="G21" s="63" t="n"/>
+      <c r="H21" s="63" t="n"/>
+      <c r="I21" s="63" t="n"/>
+      <c r="J21" s="63" t="n"/>
+      <c r="K21" s="63" t="n"/>
+      <c r="L21" s="63" t="n"/>
+      <c r="M21" s="63" t="n"/>
+      <c r="N21" s="63" t="n"/>
+      <c r="O21" s="63" t="inlineStr">
+        <is>
+          <t>vpc020</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="62" t="n"/>
@@ -2417,6 +2717,21 @@
         </is>
       </c>
       <c r="D22" s="62" t="n"/>
+      <c r="E22" s="62" t="n"/>
+      <c r="F22" s="62" t="n"/>
+      <c r="G22" s="62" t="n"/>
+      <c r="H22" s="62" t="n"/>
+      <c r="I22" s="62" t="n"/>
+      <c r="J22" s="62" t="n"/>
+      <c r="K22" s="62" t="n"/>
+      <c r="L22" s="62" t="n"/>
+      <c r="M22" s="62" t="n"/>
+      <c r="N22" s="62" t="n"/>
+      <c r="O22" s="62" t="inlineStr">
+        <is>
+          <t>vpc021</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="63" t="n"/>
@@ -2427,6 +2742,21 @@
         </is>
       </c>
       <c r="D23" s="63" t="n"/>
+      <c r="E23" s="63" t="n"/>
+      <c r="F23" s="63" t="n"/>
+      <c r="G23" s="63" t="n"/>
+      <c r="H23" s="63" t="n"/>
+      <c r="I23" s="63" t="n"/>
+      <c r="J23" s="63" t="n"/>
+      <c r="K23" s="63" t="n"/>
+      <c r="L23" s="63" t="n"/>
+      <c r="M23" s="63" t="n"/>
+      <c r="N23" s="63" t="n"/>
+      <c r="O23" s="63" t="inlineStr">
+        <is>
+          <t>vpc022</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="62" t="n"/>
@@ -2437,6 +2767,21 @@
         </is>
       </c>
       <c r="D24" s="62" t="n"/>
+      <c r="E24" s="62" t="n"/>
+      <c r="F24" s="62" t="n"/>
+      <c r="G24" s="62" t="n"/>
+      <c r="H24" s="62" t="n"/>
+      <c r="I24" s="62" t="n"/>
+      <c r="J24" s="62" t="n"/>
+      <c r="K24" s="62" t="n"/>
+      <c r="L24" s="62" t="n"/>
+      <c r="M24" s="62" t="n"/>
+      <c r="N24" s="62" t="n"/>
+      <c r="O24" s="62" t="inlineStr">
+        <is>
+          <t>vpc023</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="63" t="n"/>
@@ -2447,6 +2792,21 @@
         </is>
       </c>
       <c r="D25" s="63" t="n"/>
+      <c r="E25" s="63" t="n"/>
+      <c r="F25" s="63" t="n"/>
+      <c r="G25" s="63" t="n"/>
+      <c r="H25" s="63" t="n"/>
+      <c r="I25" s="63" t="n"/>
+      <c r="J25" s="63" t="n"/>
+      <c r="K25" s="63" t="n"/>
+      <c r="L25" s="63" t="n"/>
+      <c r="M25" s="63" t="n"/>
+      <c r="N25" s="63" t="n"/>
+      <c r="O25" s="63" t="inlineStr">
+        <is>
+          <t>vpc024</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="62" t="n"/>
@@ -2457,6 +2817,21 @@
         </is>
       </c>
       <c r="D26" s="62" t="n"/>
+      <c r="E26" s="62" t="n"/>
+      <c r="F26" s="62" t="n"/>
+      <c r="G26" s="62" t="n"/>
+      <c r="H26" s="62" t="n"/>
+      <c r="I26" s="62" t="n"/>
+      <c r="J26" s="62" t="n"/>
+      <c r="K26" s="62" t="n"/>
+      <c r="L26" s="62" t="n"/>
+      <c r="M26" s="62" t="n"/>
+      <c r="N26" s="62" t="n"/>
+      <c r="O26" s="62" t="inlineStr">
+        <is>
+          <t>vpc025</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="63" t="n"/>
@@ -2467,6 +2842,21 @@
         </is>
       </c>
       <c r="D27" s="63" t="n"/>
+      <c r="E27" s="63" t="n"/>
+      <c r="F27" s="63" t="n"/>
+      <c r="G27" s="63" t="n"/>
+      <c r="H27" s="63" t="n"/>
+      <c r="I27" s="63" t="n"/>
+      <c r="J27" s="63" t="n"/>
+      <c r="K27" s="63" t="n"/>
+      <c r="L27" s="63" t="n"/>
+      <c r="M27" s="63" t="n"/>
+      <c r="N27" s="63" t="n"/>
+      <c r="O27" s="63" t="inlineStr">
+        <is>
+          <t>vpc026</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="62" t="n"/>
@@ -2477,6 +2867,21 @@
         </is>
       </c>
       <c r="D28" s="62" t="n"/>
+      <c r="E28" s="62" t="n"/>
+      <c r="F28" s="62" t="n"/>
+      <c r="G28" s="62" t="n"/>
+      <c r="H28" s="62" t="n"/>
+      <c r="I28" s="62" t="n"/>
+      <c r="J28" s="62" t="n"/>
+      <c r="K28" s="62" t="n"/>
+      <c r="L28" s="62" t="n"/>
+      <c r="M28" s="62" t="n"/>
+      <c r="N28" s="62" t="n"/>
+      <c r="O28" s="62" t="inlineStr">
+        <is>
+          <t>vpc027</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="63" t="n"/>
@@ -2487,6 +2892,21 @@
         </is>
       </c>
       <c r="D29" s="63" t="n"/>
+      <c r="E29" s="63" t="n"/>
+      <c r="F29" s="63" t="n"/>
+      <c r="G29" s="63" t="n"/>
+      <c r="H29" s="63" t="n"/>
+      <c r="I29" s="63" t="n"/>
+      <c r="J29" s="63" t="n"/>
+      <c r="K29" s="63" t="n"/>
+      <c r="L29" s="63" t="n"/>
+      <c r="M29" s="63" t="n"/>
+      <c r="N29" s="63" t="n"/>
+      <c r="O29" s="63" t="inlineStr">
+        <is>
+          <t>vpc028</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="62" t="n"/>
@@ -2497,6 +2917,21 @@
         </is>
       </c>
       <c r="D30" s="62" t="n"/>
+      <c r="E30" s="62" t="n"/>
+      <c r="F30" s="62" t="n"/>
+      <c r="G30" s="62" t="n"/>
+      <c r="H30" s="62" t="n"/>
+      <c r="I30" s="62" t="n"/>
+      <c r="J30" s="62" t="n"/>
+      <c r="K30" s="62" t="n"/>
+      <c r="L30" s="62" t="n"/>
+      <c r="M30" s="62" t="n"/>
+      <c r="N30" s="62" t="n"/>
+      <c r="O30" s="62" t="inlineStr">
+        <is>
+          <t>vpc029</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="63" t="n"/>
@@ -2507,6 +2942,21 @@
         </is>
       </c>
       <c r="D31" s="63" t="n"/>
+      <c r="E31" s="63" t="n"/>
+      <c r="F31" s="63" t="n"/>
+      <c r="G31" s="63" t="n"/>
+      <c r="H31" s="63" t="n"/>
+      <c r="I31" s="63" t="n"/>
+      <c r="J31" s="63" t="n"/>
+      <c r="K31" s="63" t="n"/>
+      <c r="L31" s="63" t="n"/>
+      <c r="M31" s="63" t="n"/>
+      <c r="N31" s="63" t="n"/>
+      <c r="O31" s="63" t="inlineStr">
+        <is>
+          <t>vpc030</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="62" t="n"/>
@@ -2517,6 +2967,21 @@
         </is>
       </c>
       <c r="D32" s="62" t="n"/>
+      <c r="E32" s="62" t="n"/>
+      <c r="F32" s="62" t="n"/>
+      <c r="G32" s="62" t="n"/>
+      <c r="H32" s="62" t="n"/>
+      <c r="I32" s="62" t="n"/>
+      <c r="J32" s="62" t="n"/>
+      <c r="K32" s="62" t="n"/>
+      <c r="L32" s="62" t="n"/>
+      <c r="M32" s="62" t="n"/>
+      <c r="N32" s="62" t="n"/>
+      <c r="O32" s="62" t="inlineStr">
+        <is>
+          <t>vpc031</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="63" t="n"/>
@@ -2527,6 +2992,21 @@
         </is>
       </c>
       <c r="D33" s="63" t="n"/>
+      <c r="E33" s="63" t="n"/>
+      <c r="F33" s="63" t="n"/>
+      <c r="G33" s="63" t="n"/>
+      <c r="H33" s="63" t="n"/>
+      <c r="I33" s="63" t="n"/>
+      <c r="J33" s="63" t="n"/>
+      <c r="K33" s="63" t="n"/>
+      <c r="L33" s="63" t="n"/>
+      <c r="M33" s="63" t="n"/>
+      <c r="N33" s="63" t="n"/>
+      <c r="O33" s="63" t="inlineStr">
+        <is>
+          <t>vpc032</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="62" t="n"/>
@@ -2537,6 +3017,21 @@
         </is>
       </c>
       <c r="D34" s="62" t="n"/>
+      <c r="E34" s="62" t="n"/>
+      <c r="F34" s="62" t="n"/>
+      <c r="G34" s="62" t="n"/>
+      <c r="H34" s="62" t="n"/>
+      <c r="I34" s="62" t="n"/>
+      <c r="J34" s="62" t="n"/>
+      <c r="K34" s="62" t="n"/>
+      <c r="L34" s="62" t="n"/>
+      <c r="M34" s="62" t="n"/>
+      <c r="N34" s="62" t="n"/>
+      <c r="O34" s="62" t="inlineStr">
+        <is>
+          <t>vpc033</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="63" t="n"/>
@@ -2547,6 +3042,21 @@
         </is>
       </c>
       <c r="D35" s="63" t="n"/>
+      <c r="E35" s="63" t="n"/>
+      <c r="F35" s="63" t="n"/>
+      <c r="G35" s="63" t="n"/>
+      <c r="H35" s="63" t="n"/>
+      <c r="I35" s="63" t="n"/>
+      <c r="J35" s="63" t="n"/>
+      <c r="K35" s="63" t="n"/>
+      <c r="L35" s="63" t="n"/>
+      <c r="M35" s="63" t="n"/>
+      <c r="N35" s="63" t="n"/>
+      <c r="O35" s="63" t="inlineStr">
+        <is>
+          <t>vpc034</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="62" t="n"/>
@@ -2557,6 +3067,21 @@
         </is>
       </c>
       <c r="D36" s="62" t="n"/>
+      <c r="E36" s="62" t="n"/>
+      <c r="F36" s="62" t="n"/>
+      <c r="G36" s="62" t="n"/>
+      <c r="H36" s="62" t="n"/>
+      <c r="I36" s="62" t="n"/>
+      <c r="J36" s="62" t="n"/>
+      <c r="K36" s="62" t="n"/>
+      <c r="L36" s="62" t="n"/>
+      <c r="M36" s="62" t="n"/>
+      <c r="N36" s="62" t="n"/>
+      <c r="O36" s="62" t="inlineStr">
+        <is>
+          <t>vpc035</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="63" t="n"/>
@@ -2567,6 +3092,21 @@
         </is>
       </c>
       <c r="D37" s="63" t="n"/>
+      <c r="E37" s="63" t="n"/>
+      <c r="F37" s="63" t="n"/>
+      <c r="G37" s="63" t="n"/>
+      <c r="H37" s="63" t="n"/>
+      <c r="I37" s="63" t="n"/>
+      <c r="J37" s="63" t="n"/>
+      <c r="K37" s="63" t="n"/>
+      <c r="L37" s="63" t="n"/>
+      <c r="M37" s="63" t="n"/>
+      <c r="N37" s="63" t="n"/>
+      <c r="O37" s="63" t="inlineStr">
+        <is>
+          <t>vpc036</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="62" t="n"/>
@@ -2577,6 +3117,21 @@
         </is>
       </c>
       <c r="D38" s="62" t="n"/>
+      <c r="E38" s="62" t="n"/>
+      <c r="F38" s="62" t="n"/>
+      <c r="G38" s="62" t="n"/>
+      <c r="H38" s="62" t="n"/>
+      <c r="I38" s="62" t="n"/>
+      <c r="J38" s="62" t="n"/>
+      <c r="K38" s="62" t="n"/>
+      <c r="L38" s="62" t="n"/>
+      <c r="M38" s="62" t="n"/>
+      <c r="N38" s="62" t="n"/>
+      <c r="O38" s="62" t="inlineStr">
+        <is>
+          <t>vpc037</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="63" t="n"/>
@@ -2587,6 +3142,21 @@
         </is>
       </c>
       <c r="D39" s="63" t="n"/>
+      <c r="E39" s="63" t="n"/>
+      <c r="F39" s="63" t="n"/>
+      <c r="G39" s="63" t="n"/>
+      <c r="H39" s="63" t="n"/>
+      <c r="I39" s="63" t="n"/>
+      <c r="J39" s="63" t="n"/>
+      <c r="K39" s="63" t="n"/>
+      <c r="L39" s="63" t="n"/>
+      <c r="M39" s="63" t="n"/>
+      <c r="N39" s="63" t="n"/>
+      <c r="O39" s="63" t="inlineStr">
+        <is>
+          <t>vpc038</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="62" t="n"/>
@@ -2597,6 +3167,21 @@
         </is>
       </c>
       <c r="D40" s="62" t="n"/>
+      <c r="E40" s="62" t="n"/>
+      <c r="F40" s="62" t="n"/>
+      <c r="G40" s="62" t="n"/>
+      <c r="H40" s="62" t="n"/>
+      <c r="I40" s="62" t="n"/>
+      <c r="J40" s="62" t="n"/>
+      <c r="K40" s="62" t="n"/>
+      <c r="L40" s="62" t="n"/>
+      <c r="M40" s="62" t="n"/>
+      <c r="N40" s="62" t="n"/>
+      <c r="O40" s="62" t="inlineStr">
+        <is>
+          <t>vpc039</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="63" t="n"/>
@@ -2607,6 +3192,21 @@
         </is>
       </c>
       <c r="D41" s="63" t="n"/>
+      <c r="E41" s="63" t="n"/>
+      <c r="F41" s="63" t="n"/>
+      <c r="G41" s="63" t="n"/>
+      <c r="H41" s="63" t="n"/>
+      <c r="I41" s="63" t="n"/>
+      <c r="J41" s="63" t="n"/>
+      <c r="K41" s="63" t="n"/>
+      <c r="L41" s="63" t="n"/>
+      <c r="M41" s="63" t="n"/>
+      <c r="N41" s="63" t="n"/>
+      <c r="O41" s="63" t="inlineStr">
+        <is>
+          <t>vpc040</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="62" t="n"/>
@@ -2617,6 +3217,21 @@
         </is>
       </c>
       <c r="D42" s="62" t="n"/>
+      <c r="E42" s="62" t="n"/>
+      <c r="F42" s="62" t="n"/>
+      <c r="G42" s="62" t="n"/>
+      <c r="H42" s="62" t="n"/>
+      <c r="I42" s="62" t="n"/>
+      <c r="J42" s="62" t="n"/>
+      <c r="K42" s="62" t="n"/>
+      <c r="L42" s="62" t="n"/>
+      <c r="M42" s="62" t="n"/>
+      <c r="N42" s="62" t="n"/>
+      <c r="O42" s="62" t="inlineStr">
+        <is>
+          <t>vpc041</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="63" t="n"/>
@@ -2627,6 +3242,21 @@
         </is>
       </c>
       <c r="D43" s="63" t="n"/>
+      <c r="E43" s="63" t="n"/>
+      <c r="F43" s="63" t="n"/>
+      <c r="G43" s="63" t="n"/>
+      <c r="H43" s="63" t="n"/>
+      <c r="I43" s="63" t="n"/>
+      <c r="J43" s="63" t="n"/>
+      <c r="K43" s="63" t="n"/>
+      <c r="L43" s="63" t="n"/>
+      <c r="M43" s="63" t="n"/>
+      <c r="N43" s="63" t="n"/>
+      <c r="O43" s="63" t="inlineStr">
+        <is>
+          <t>vpc042</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="62" t="n"/>
@@ -2637,6 +3267,21 @@
         </is>
       </c>
       <c r="D44" s="62" t="n"/>
+      <c r="E44" s="62" t="n"/>
+      <c r="F44" s="62" t="n"/>
+      <c r="G44" s="62" t="n"/>
+      <c r="H44" s="62" t="n"/>
+      <c r="I44" s="62" t="n"/>
+      <c r="J44" s="62" t="n"/>
+      <c r="K44" s="62" t="n"/>
+      <c r="L44" s="62" t="n"/>
+      <c r="M44" s="62" t="n"/>
+      <c r="N44" s="62" t="n"/>
+      <c r="O44" s="62" t="inlineStr">
+        <is>
+          <t>vpc043</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="63" t="n"/>
@@ -2647,6 +3292,21 @@
         </is>
       </c>
       <c r="D45" s="63" t="n"/>
+      <c r="E45" s="63" t="n"/>
+      <c r="F45" s="63" t="n"/>
+      <c r="G45" s="63" t="n"/>
+      <c r="H45" s="63" t="n"/>
+      <c r="I45" s="63" t="n"/>
+      <c r="J45" s="63" t="n"/>
+      <c r="K45" s="63" t="n"/>
+      <c r="L45" s="63" t="n"/>
+      <c r="M45" s="63" t="n"/>
+      <c r="N45" s="63" t="n"/>
+      <c r="O45" s="63" t="inlineStr">
+        <is>
+          <t>vpc044</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="62" t="n"/>
@@ -2657,6 +3317,21 @@
         </is>
       </c>
       <c r="D46" s="62" t="n"/>
+      <c r="E46" s="62" t="n"/>
+      <c r="F46" s="62" t="n"/>
+      <c r="G46" s="62" t="n"/>
+      <c r="H46" s="62" t="n"/>
+      <c r="I46" s="62" t="n"/>
+      <c r="J46" s="62" t="n"/>
+      <c r="K46" s="62" t="n"/>
+      <c r="L46" s="62" t="n"/>
+      <c r="M46" s="62" t="n"/>
+      <c r="N46" s="62" t="n"/>
+      <c r="O46" s="62" t="inlineStr">
+        <is>
+          <t>vpc045</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="63" t="n"/>
@@ -2667,6 +3342,21 @@
         </is>
       </c>
       <c r="D47" s="63" t="n"/>
+      <c r="E47" s="63" t="n"/>
+      <c r="F47" s="63" t="n"/>
+      <c r="G47" s="63" t="n"/>
+      <c r="H47" s="63" t="n"/>
+      <c r="I47" s="63" t="n"/>
+      <c r="J47" s="63" t="n"/>
+      <c r="K47" s="63" t="n"/>
+      <c r="L47" s="63" t="n"/>
+      <c r="M47" s="63" t="n"/>
+      <c r="N47" s="63" t="n"/>
+      <c r="O47" s="63" t="inlineStr">
+        <is>
+          <t>vpc046</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="62" t="n"/>
@@ -2677,6 +3367,21 @@
         </is>
       </c>
       <c r="D48" s="62" t="n"/>
+      <c r="E48" s="62" t="n"/>
+      <c r="F48" s="62" t="n"/>
+      <c r="G48" s="62" t="n"/>
+      <c r="H48" s="62" t="n"/>
+      <c r="I48" s="62" t="n"/>
+      <c r="J48" s="62" t="n"/>
+      <c r="K48" s="62" t="n"/>
+      <c r="L48" s="62" t="n"/>
+      <c r="M48" s="62" t="n"/>
+      <c r="N48" s="62" t="n"/>
+      <c r="O48" s="62" t="inlineStr">
+        <is>
+          <t>vpc047</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="63" t="n"/>
@@ -2687,6 +3392,21 @@
         </is>
       </c>
       <c r="D49" s="63" t="n"/>
+      <c r="E49" s="63" t="n"/>
+      <c r="F49" s="63" t="n"/>
+      <c r="G49" s="63" t="n"/>
+      <c r="H49" s="63" t="n"/>
+      <c r="I49" s="63" t="n"/>
+      <c r="J49" s="63" t="n"/>
+      <c r="K49" s="63" t="n"/>
+      <c r="L49" s="63" t="n"/>
+      <c r="M49" s="63" t="n"/>
+      <c r="N49" s="63" t="n"/>
+      <c r="O49" s="63" t="inlineStr">
+        <is>
+          <t>vpc048</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="62" t="n"/>
@@ -2697,6 +3417,21 @@
         </is>
       </c>
       <c r="D50" s="62" t="n"/>
+      <c r="E50" s="62" t="n"/>
+      <c r="F50" s="62" t="n"/>
+      <c r="G50" s="62" t="n"/>
+      <c r="H50" s="62" t="n"/>
+      <c r="I50" s="62" t="n"/>
+      <c r="J50" s="62" t="n"/>
+      <c r="K50" s="62" t="n"/>
+      <c r="L50" s="62" t="n"/>
+      <c r="M50" s="62" t="n"/>
+      <c r="N50" s="62" t="n"/>
+      <c r="O50" s="62" t="inlineStr">
+        <is>
+          <t>vpc049</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="63" t="n"/>
@@ -2707,6 +3442,21 @@
         </is>
       </c>
       <c r="D51" s="63" t="n"/>
+      <c r="E51" s="63" t="n"/>
+      <c r="F51" s="63" t="n"/>
+      <c r="G51" s="63" t="n"/>
+      <c r="H51" s="63" t="n"/>
+      <c r="I51" s="63" t="n"/>
+      <c r="J51" s="63" t="n"/>
+      <c r="K51" s="63" t="n"/>
+      <c r="L51" s="63" t="n"/>
+      <c r="M51" s="63" t="n"/>
+      <c r="N51" s="63" t="n"/>
+      <c r="O51" s="63" t="inlineStr">
+        <is>
+          <t>vpc050</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="62" t="n"/>
@@ -2717,6 +3467,21 @@
         </is>
       </c>
       <c r="D52" s="62" t="n"/>
+      <c r="E52" s="62" t="n"/>
+      <c r="F52" s="62" t="n"/>
+      <c r="G52" s="62" t="n"/>
+      <c r="H52" s="62" t="n"/>
+      <c r="I52" s="62" t="n"/>
+      <c r="J52" s="62" t="n"/>
+      <c r="K52" s="62" t="n"/>
+      <c r="L52" s="62" t="n"/>
+      <c r="M52" s="62" t="n"/>
+      <c r="N52" s="62" t="n"/>
+      <c r="O52" s="62" t="inlineStr">
+        <is>
+          <t>vpc051</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="63" t="n"/>
@@ -2727,6 +3492,21 @@
         </is>
       </c>
       <c r="D53" s="63" t="n"/>
+      <c r="E53" s="63" t="n"/>
+      <c r="F53" s="63" t="n"/>
+      <c r="G53" s="63" t="n"/>
+      <c r="H53" s="63" t="n"/>
+      <c r="I53" s="63" t="n"/>
+      <c r="J53" s="63" t="n"/>
+      <c r="K53" s="63" t="n"/>
+      <c r="L53" s="63" t="n"/>
+      <c r="M53" s="63" t="n"/>
+      <c r="N53" s="63" t="n"/>
+      <c r="O53" s="63" t="inlineStr">
+        <is>
+          <t>vpc052</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="62" t="n"/>
@@ -2737,6 +3517,21 @@
         </is>
       </c>
       <c r="D54" s="62" t="n"/>
+      <c r="E54" s="62" t="n"/>
+      <c r="F54" s="62" t="n"/>
+      <c r="G54" s="62" t="n"/>
+      <c r="H54" s="62" t="n"/>
+      <c r="I54" s="62" t="n"/>
+      <c r="J54" s="62" t="n"/>
+      <c r="K54" s="62" t="n"/>
+      <c r="L54" s="62" t="n"/>
+      <c r="M54" s="62" t="n"/>
+      <c r="N54" s="62" t="n"/>
+      <c r="O54" s="62" t="inlineStr">
+        <is>
+          <t>vpc053</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="63" t="n"/>
@@ -2747,6 +3542,21 @@
         </is>
       </c>
       <c r="D55" s="63" t="n"/>
+      <c r="E55" s="63" t="n"/>
+      <c r="F55" s="63" t="n"/>
+      <c r="G55" s="63" t="n"/>
+      <c r="H55" s="63" t="n"/>
+      <c r="I55" s="63" t="n"/>
+      <c r="J55" s="63" t="n"/>
+      <c r="K55" s="63" t="n"/>
+      <c r="L55" s="63" t="n"/>
+      <c r="M55" s="63" t="n"/>
+      <c r="N55" s="63" t="n"/>
+      <c r="O55" s="63" t="inlineStr">
+        <is>
+          <t>vpc054</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="62" t="n"/>
@@ -2757,6 +3567,21 @@
         </is>
       </c>
       <c r="D56" s="62" t="n"/>
+      <c r="E56" s="62" t="n"/>
+      <c r="F56" s="62" t="n"/>
+      <c r="G56" s="62" t="n"/>
+      <c r="H56" s="62" t="n"/>
+      <c r="I56" s="62" t="n"/>
+      <c r="J56" s="62" t="n"/>
+      <c r="K56" s="62" t="n"/>
+      <c r="L56" s="62" t="n"/>
+      <c r="M56" s="62" t="n"/>
+      <c r="N56" s="62" t="n"/>
+      <c r="O56" s="62" t="inlineStr">
+        <is>
+          <t>vpc055</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="63" t="n"/>
@@ -2767,6 +3592,21 @@
         </is>
       </c>
       <c r="D57" s="63" t="n"/>
+      <c r="E57" s="63" t="n"/>
+      <c r="F57" s="63" t="n"/>
+      <c r="G57" s="63" t="n"/>
+      <c r="H57" s="63" t="n"/>
+      <c r="I57" s="63" t="n"/>
+      <c r="J57" s="63" t="n"/>
+      <c r="K57" s="63" t="n"/>
+      <c r="L57" s="63" t="n"/>
+      <c r="M57" s="63" t="n"/>
+      <c r="N57" s="63" t="n"/>
+      <c r="O57" s="63" t="inlineStr">
+        <is>
+          <t>vpc056</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="62" t="n"/>
@@ -2777,6 +3617,21 @@
         </is>
       </c>
       <c r="D58" s="62" t="n"/>
+      <c r="E58" s="62" t="n"/>
+      <c r="F58" s="62" t="n"/>
+      <c r="G58" s="62" t="n"/>
+      <c r="H58" s="62" t="n"/>
+      <c r="I58" s="62" t="n"/>
+      <c r="J58" s="62" t="n"/>
+      <c r="K58" s="62" t="n"/>
+      <c r="L58" s="62" t="n"/>
+      <c r="M58" s="62" t="n"/>
+      <c r="N58" s="62" t="n"/>
+      <c r="O58" s="62" t="inlineStr">
+        <is>
+          <t>vpc057</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="63" t="n"/>
@@ -2787,6 +3642,21 @@
         </is>
       </c>
       <c r="D59" s="63" t="n"/>
+      <c r="E59" s="63" t="n"/>
+      <c r="F59" s="63" t="n"/>
+      <c r="G59" s="63" t="n"/>
+      <c r="H59" s="63" t="n"/>
+      <c r="I59" s="63" t="n"/>
+      <c r="J59" s="63" t="n"/>
+      <c r="K59" s="63" t="n"/>
+      <c r="L59" s="63" t="n"/>
+      <c r="M59" s="63" t="n"/>
+      <c r="N59" s="63" t="n"/>
+      <c r="O59" s="63" t="inlineStr">
+        <is>
+          <t>vpc058</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="62" t="n"/>
@@ -2797,6 +3667,21 @@
         </is>
       </c>
       <c r="D60" s="62" t="n"/>
+      <c r="E60" s="62" t="n"/>
+      <c r="F60" s="62" t="n"/>
+      <c r="G60" s="62" t="n"/>
+      <c r="H60" s="62" t="n"/>
+      <c r="I60" s="62" t="n"/>
+      <c r="J60" s="62" t="n"/>
+      <c r="K60" s="62" t="n"/>
+      <c r="L60" s="62" t="n"/>
+      <c r="M60" s="62" t="n"/>
+      <c r="N60" s="62" t="n"/>
+      <c r="O60" s="62" t="inlineStr">
+        <is>
+          <t>vpc059</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="63" t="n"/>
@@ -2807,6 +3692,21 @@
         </is>
       </c>
       <c r="D61" s="63" t="n"/>
+      <c r="E61" s="63" t="n"/>
+      <c r="F61" s="63" t="n"/>
+      <c r="G61" s="63" t="n"/>
+      <c r="H61" s="63" t="n"/>
+      <c r="I61" s="63" t="n"/>
+      <c r="J61" s="63" t="n"/>
+      <c r="K61" s="63" t="n"/>
+      <c r="L61" s="63" t="n"/>
+      <c r="M61" s="63" t="n"/>
+      <c r="N61" s="63" t="n"/>
+      <c r="O61" s="63" t="inlineStr">
+        <is>
+          <t>vpc060</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>